<commit_message>
Crud MS2 insya Allah regse
</commit_message>
<xml_diff>
--- a/assets/file/format_oscrms_ms2.xlsx
+++ b/assets/file/format_oscrms_ms2.xlsx
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,10 +1089,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4">
         <v>0.03</v>

</xml_diff>